<commit_message>
actualizacion del cronograma de actividades
</commit_message>
<xml_diff>
--- a/Cronograma de actividades_RestauranteSazónDeLaAbuela.xlsx
+++ b/Cronograma de actividades_RestauranteSazónDeLaAbuela.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoel B\Desktop\Proyecto-2\Proyecto 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoel B\Desktop\proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -129,16 +129,16 @@
     <t xml:space="preserve">Restaurante el sazón de la abuela </t>
   </si>
   <si>
-    <t xml:space="preserve">Determinar el diseño que desa el cliente </t>
-  </si>
-  <si>
     <t>Programador</t>
   </si>
   <si>
-    <t>web master</t>
-  </si>
-  <si>
     <t>Gerente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determinar el diseño que desea el cliente </t>
+  </si>
+  <si>
+    <t>Web Master</t>
   </si>
 </sst>
 </file>
@@ -251,9 +251,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,6 +264,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -566,8 +566,8 @@
     <col min="7" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -592,48 +592,48 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
-        <v>34</v>
+      <c r="C3" s="6">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>3</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>34</v>
+      <c r="E4" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>5</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -641,30 +641,30 @@
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7">
-        <v>4</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6">
         <v>3</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6">
         <v>5</v>
       </c>
-      <c r="D7" s="7">
-        <v>4</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="6">
+        <v>4</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -672,243 +672,247 @@
       <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="7">
-        <v>4</v>
-      </c>
-      <c r="D9" s="7">
-        <v>4</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>34</v>
+      <c r="C9" s="6">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6">
+        <v>4</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7">
-        <v>4</v>
-      </c>
-      <c r="D10" s="7">
-        <v>4</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>34</v>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6">
+        <v>4</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="7">
-        <v>4</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>34</v>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>3</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>5</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>32</v>
+      <c r="E12" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>10</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>9</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>33</v>
+      <c r="E14" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>15</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>11</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>33</v>
+      <c r="E15" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>15</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>33</v>
+      <c r="E16" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>30</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>13</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>33</v>
+      <c r="E18" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
-        <v>33</v>
+      <c r="C19" s="6">
+        <v>30</v>
+      </c>
+      <c r="D19" s="6">
+        <v>15</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>30</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>15</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>32</v>
+      <c r="E20" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>7</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>17</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>32</v>
+      <c r="E22" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>7</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>17</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -916,51 +920,51 @@
       <c r="A24" s="4">
         <v>21</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>5</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>17</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>32</v>
+      <c r="E24" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>22</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="7">
-        <v>4</v>
-      </c>
-      <c r="D25" s="7">
+      <c r="C25" s="6">
+        <v>4</v>
+      </c>
+      <c r="D25" s="6">
         <v>17</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>32</v>
+      <c r="E25" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>23</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>1</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>18</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>34</v>
+      <c r="E26" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
actulizacion cronograma de actividades 2
</commit_message>
<xml_diff>
--- a/Cronograma de actividades_RestauranteSazónDeLaAbuela.xlsx
+++ b/Cronograma de actividades_RestauranteSazónDeLaAbuela.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Nombre de las tareas</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Web Master</t>
+  </si>
+  <si>
+    <t>programador-Analista</t>
   </si>
 </sst>
 </file>
@@ -237,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,6 +270,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -552,7 +558,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -912,8 +918,8 @@
       <c r="D23" s="6">
         <v>17</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>29</v>
+      <c r="E23" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
actulizacion C.A., se agrega cronograma de actividades Gant project
</commit_message>
<xml_diff>
--- a/Cronograma de actividades_RestauranteSazónDeLaAbuela.xlsx
+++ b/Cronograma de actividades_RestauranteSazónDeLaAbuela.xlsx
@@ -268,11 +268,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -572,8 +572,8 @@
     <col min="7" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>30</v>
       </c>
     </row>
@@ -918,7 +918,7 @@
       <c r="D23" s="6">
         <v>17</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>